<commit_message>
- Hooked up way to keep track of the player's current power state - Hooked up the small mario image frames
</commit_message>
<xml_diff>
--- a/spritesheet_coords.xlsx
+++ b/spritesheet_coords.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>x</t>
   </si>
@@ -45,6 +45,36 @@
   </si>
   <si>
     <t>start at 0</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>walk_r1</t>
+  </si>
+  <si>
+    <t>walk_r2</t>
+  </si>
+  <si>
+    <t>walk_r3</t>
+  </si>
+  <si>
+    <t>jump_r</t>
+  </si>
+  <si>
+    <t>walk_l1</t>
+  </si>
+  <si>
+    <t>walk_l2</t>
+  </si>
+  <si>
+    <t>walk_l3</t>
+  </si>
+  <si>
+    <t>jump_l</t>
   </si>
 </sst>
 </file>
@@ -80,8 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,20 +395,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:H11"/>
+  <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
@@ -389,9 +438,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4">
+        <v>223</v>
+      </c>
+      <c r="D4">
+        <v>43</v>
       </c>
       <c r="E4">
         <v>238</v>
@@ -406,9 +461,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>4</v>
+      </c>
+      <c r="C5">
+        <v>276</v>
+      </c>
+      <c r="D5">
+        <v>43</v>
       </c>
       <c r="E5">
         <v>257</v>
@@ -416,44 +477,141 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>291</v>
+      </c>
       <c r="E6">
         <f>E5+G$4+1</f>
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>305</v>
+      </c>
       <c r="E7">
         <f t="shared" ref="E7:E11" si="0">E6+G$4+1</f>
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>321</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E9">
         <f t="shared" si="0"/>
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>355</v>
+      </c>
+      <c r="D10">
+        <v>43</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>352</v>
       </c>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>142</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>371</v>
       </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>208</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>194</v>
+      </c>
+      <c r="G14">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>178</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Added way to transition from small to big
</commit_message>
<xml_diff>
--- a/spritesheet_coords.xlsx
+++ b/spritesheet_coords.xlsx
@@ -110,11 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,15 +396,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H15"/>
+  <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
@@ -413,12 +414,12 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -438,7 +439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -461,7 +462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -484,7 +485,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -496,7 +497,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -507,8 +508,9 @@
         <f t="shared" ref="E7:E11" si="0">E6+G$4+1</f>
         <v>295</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -520,13 +522,13 @@
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E9">
         <f t="shared" si="0"/>
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -547,7 +549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -565,7 +567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -579,7 +581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -593,7 +595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>

</xml_diff>